<commit_message>
Update transaction entity and xlsx file
</commit_message>
<xml_diff>
--- a/backend/src/transactions/transactions.xlsx
+++ b/backend/src/transactions/transactions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harel\Elazar Harel\taxmyself\taxmyself-dev\backend\src\transactions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E1692A5C-03B4-4105-8C52-FC43287AF257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB5D4636-4AAD-4F4F-864A-BB49DFEEB0D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="transactions" sheetId="1" r:id="rId1"/>
@@ -20,87 +20,84 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
   <si>
     <t>שם העסק</t>
   </si>
   <si>
-    <t>תאריך חיוב</t>
-  </si>
-  <si>
-    <t>תאריך תשלום</t>
-  </si>
-  <si>
     <t>סכום</t>
   </si>
   <si>
-    <t>קטגוריה</t>
-  </si>
-  <si>
-    <t>העברה דיגי700</t>
-  </si>
-  <si>
-    <t>הוצאות לא תזרימיות</t>
-  </si>
-  <si>
-    <t>העברה לח.נוסף</t>
-  </si>
-  <si>
-    <t>הכנסות לא תזרימיות</t>
-  </si>
-  <si>
-    <t>המרת מטח</t>
-  </si>
-  <si>
-    <t>מאוצר החייל-י</t>
-  </si>
-  <si>
     <t>מנוי riseup</t>
   </si>
   <si>
-    <t>RiseUp</t>
-  </si>
-  <si>
-    <t>איילון ביטוח חיים וב</t>
-  </si>
-  <si>
-    <t>ביטוח</t>
-  </si>
-  <si>
-    <t>הכשרה GO ביטוח-צמרת</t>
-  </si>
-  <si>
     <t>הכשרה חובה אקספרס-צמ</t>
   </si>
   <si>
-    <t>קרן מכבי- חיוב</t>
-  </si>
-  <si>
-    <t>מנורה מבטחים פנסיה וגמל בעמ</t>
-  </si>
-  <si>
     <t>מגדל חיים/בריאות</t>
   </si>
   <si>
-    <t>כלל רכב/דירה/עסק</t>
-  </si>
-  <si>
-    <t>ביטוח לאומי ספק הוק</t>
-  </si>
-  <si>
     <t>ביטוח לאומי</t>
   </si>
   <si>
     <t>אדיר גז</t>
   </si>
   <si>
-    <t>גז</t>
+    <t>אמצעי זיהוי התשלום</t>
+  </si>
+  <si>
+    <t>תאריך התשלום</t>
+  </si>
+  <si>
+    <t>תאריך החיוב בחשבון</t>
+  </si>
+  <si>
+    <t>רמי לוי</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>מופת מילואים</t>
+  </si>
+  <si>
+    <t>מכבי שירותי בריאות</t>
+  </si>
+  <si>
+    <t>איילון ביטוח חיים</t>
+  </si>
+  <si>
+    <t>תרומה חסדי נעמי</t>
+  </si>
+  <si>
+    <t>משכורת אינטל</t>
+  </si>
+  <si>
+    <t>מנורה מבטחים פנסיה</t>
+  </si>
+  <si>
+    <t>ביטוח ישיר - רכב</t>
+  </si>
+  <si>
+    <t>קצבת ילדים</t>
+  </si>
+  <si>
+    <t>צילומינציה</t>
+  </si>
+  <si>
+    <t>20-521-567890</t>
+  </si>
+  <si>
+    <t>10-680-335679</t>
+  </si>
+  <si>
+    <t>5678</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -596,9 +593,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - הדגשה1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -658,9 +661,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא של Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -698,7 +701,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -804,7 +807,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -946,24 +949,26 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="10.5" customWidth="1"/>
+    <col min="1" max="1" width="27.5" customWidth="1"/>
+    <col min="2" max="2" width="19.296875" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="23.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -971,308 +976,343 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1">
-        <v>45306</v>
+        <v>10</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1234</v>
       </c>
       <c r="C2" s="1">
         <v>45306</v>
       </c>
-      <c r="D2">
-        <v>-24000</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
+      <c r="D2" s="1">
+        <v>45306</v>
+      </c>
+      <c r="E2">
+        <v>-735.46</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1">
-        <v>45308</v>
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="C3" s="1">
-        <v>45308</v>
-      </c>
-      <c r="D3">
-        <v>-35000</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
+        <v>45306</v>
+      </c>
+      <c r="D3" s="1">
+        <v>45306</v>
+      </c>
+      <c r="E3">
+        <v>-289.67</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1">
-        <v>45306</v>
+        <v>12</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="C4" s="1">
-        <v>45306</v>
-      </c>
-      <c r="D4">
-        <v>24000</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
+        <v>45308</v>
+      </c>
+      <c r="D4" s="1">
+        <v>45308</v>
+      </c>
+      <c r="E4">
+        <v>1500</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="1">
-        <v>45306</v>
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C5" s="1">
-        <v>45306</v>
-      </c>
-      <c r="D5">
-        <v>39712.53</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
+        <v>45324</v>
+      </c>
+      <c r="D5" s="1">
+        <v>45324</v>
+      </c>
+      <c r="E5">
+        <v>-1300</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1">
-        <v>45308</v>
+        <v>13</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="C6" s="1">
-        <v>45308</v>
-      </c>
-      <c r="D6">
-        <v>35000</v>
-      </c>
-      <c r="E6" t="s">
-        <v>8</v>
+        <v>45293</v>
+      </c>
+      <c r="D6" s="1">
+        <v>45293</v>
+      </c>
+      <c r="E6">
+        <v>-257.49</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="1">
-        <v>45292</v>
-      </c>
       <c r="C7" s="1">
-        <v>45324</v>
-      </c>
-      <c r="D7">
+        <v>45293</v>
+      </c>
+      <c r="D7" s="1">
+        <v>45293</v>
+      </c>
+      <c r="E7">
         <v>-45</v>
-      </c>
-      <c r="E7" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="1">
-        <v>45288</v>
+        <v>14</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="C8" s="1">
         <v>45293</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
+        <v>45293</v>
+      </c>
+      <c r="E8">
         <v>-56.62</v>
-      </c>
-      <c r="E8" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="1">
-        <v>45292</v>
+      <c r="B9" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="C9" s="1">
-        <v>45293</v>
-      </c>
-      <c r="D9">
-        <v>-334.5</v>
-      </c>
-      <c r="E9" t="s">
-        <v>14</v>
+        <v>45324</v>
+      </c>
+      <c r="D9" s="1">
+        <v>45324</v>
+      </c>
+      <c r="E9">
+        <v>-350</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="1">
-        <v>45292</v>
+        <v>3</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="C10" s="1">
-        <v>45293</v>
-      </c>
-      <c r="D10">
+        <v>45324</v>
+      </c>
+      <c r="D10" s="1">
+        <v>45324</v>
+      </c>
+      <c r="E10">
         <v>-144</v>
-      </c>
-      <c r="E10" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="1">
-        <v>45293</v>
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="C11" s="1">
-        <v>45324</v>
-      </c>
-      <c r="D11">
+        <v>45333</v>
+      </c>
+      <c r="D11" s="1">
+        <v>45333</v>
+      </c>
+      <c r="E11">
         <v>-327.48</v>
-      </c>
-      <c r="E11" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="1">
-        <v>45294</v>
+        <v>16</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="C12" s="1">
         <v>45324</v>
       </c>
-      <c r="D12">
-        <v>-22.94</v>
-      </c>
-      <c r="E12" t="s">
-        <v>14</v>
+      <c r="D12" s="1">
+        <v>45324</v>
+      </c>
+      <c r="E12">
+        <v>15700</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="1">
-        <v>45306</v>
+        <v>17</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C13" s="1">
-        <v>45333</v>
-      </c>
-      <c r="D13">
+        <v>45324</v>
+      </c>
+      <c r="D13" s="1">
+        <v>45324</v>
+      </c>
+      <c r="E13">
         <v>-439.47</v>
-      </c>
-      <c r="E13" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="1">
-        <v>45312</v>
+        <v>4</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="C14" s="1">
         <v>45324</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="1">
+        <v>45324</v>
+      </c>
+      <c r="E14">
         <v>-11.97</v>
-      </c>
-      <c r="E14" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="1">
-        <v>45312</v>
+        <v>4</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="C15" s="1">
-        <v>45324</v>
-      </c>
-      <c r="D15">
+        <v>45333</v>
+      </c>
+      <c r="D15" s="1">
+        <v>45333</v>
+      </c>
+      <c r="E15">
         <v>-23.35</v>
-      </c>
-      <c r="E15" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="1">
-        <v>45319</v>
+        <v>18</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="C16" s="1">
         <v>45324</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="1">
+        <v>45324</v>
+      </c>
+      <c r="E16">
         <v>-190.25</v>
-      </c>
-      <c r="E16" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="1">
-        <v>45304</v>
-      </c>
       <c r="C17" s="1">
-        <v>45333</v>
-      </c>
-      <c r="D17">
-        <v>-485</v>
-      </c>
-      <c r="E17" t="s">
-        <v>22</v>
+        <v>45332</v>
+      </c>
+      <c r="D17" s="1">
+        <v>45332</v>
+      </c>
+      <c r="E17">
+        <v>550</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="1">
-        <v>45300</v>
-      </c>
       <c r="C18" s="1">
-        <v>45324</v>
-      </c>
-      <c r="D18">
+        <v>45636</v>
+      </c>
+      <c r="D18" s="1">
+        <v>45636</v>
+      </c>
+      <c r="E18">
         <v>-323.39999999999998</v>
       </c>
-      <c r="E18" t="s">
-        <v>24</v>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="3">
+        <v>5670</v>
+      </c>
+      <c r="C19" s="1">
+        <v>45332</v>
+      </c>
+      <c r="D19" s="1">
+        <v>45332</v>
+      </c>
+      <c r="E19">
+        <v>-170</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="3">
+        <v>5670</v>
+      </c>
+      <c r="C20" s="1">
+        <v>45337</v>
+      </c>
+      <c r="D20" s="1">
+        <v>45337</v>
+      </c>
+      <c r="E20">
+        <v>-300</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>